<commit_message>
Update to work with the latest version of SFDC
</commit_message>
<xml_diff>
--- a/TC_CreateNewLead/Main.rvl.xlsx
+++ b/TC_CreateNewLead/Main.rvl.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="132">
   <si>
     <t>Flow</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>SearchTable</t>
+  </si>
+  <si>
+    <t>SelectComboboxItem</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="711">
+  <borders count="713">
     <border>
       <left/>
       <right/>
@@ -1145,11 +1148,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="711">
+  <cellXfs count="713">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -1861,6 +1866,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="708" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="709" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="710" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="711" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="712" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2377,10 +2384,10 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="E29" t="s">
         <v>49</v>
@@ -2393,7 +2400,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="183"/>
+      <c r="A30" s="711"/>
       <c r="B30" t="s">
         <v>42</v>
       </c>
@@ -2413,10 +2420,10 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="E31" t="s">
         <v>49</v>
@@ -2429,7 +2436,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="185"/>
+      <c r="A32" s="712"/>
       <c r="B32" t="s">
         <v>42</v>
       </c>

</xml_diff>